<commit_message>
Chat system operational, begun work on issuing challenges, need to devise how to accept and launch a game window as well as create another server for each game.
</commit_message>
<xml_diff>
--- a/FINAL_PROJECT_Gerrit_Kat_04_18_2022.xlsx
+++ b/FINAL_PROJECT_Gerrit_Kat_04_18_2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\School Projects\PROG 280 - Advanced Programming\Blackjack-Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E56A77C2-741F-4B63-871C-16C6BB0C3EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51692EB0-C141-4B82-8579-5DED2E5250D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
   <si>
     <t>Task</t>
   </si>
@@ -142,37 +142,46 @@
     <t>Establish a connection between players</t>
   </si>
   <si>
-    <t>Create User Classes</t>
-  </si>
-  <si>
-    <t>User Accounts</t>
-  </si>
-  <si>
     <t>2 hours</t>
   </si>
   <si>
     <t>Create Card/Deck Classes</t>
   </si>
   <si>
-    <t>Created card class with constructor, created deck with option to add cards and method to shuffle the deck.</t>
-  </si>
-  <si>
     <t>30 mins</t>
   </si>
   <si>
     <t>Add classes to manage the cards in a deck and shuffle them for randomization.</t>
   </si>
   <si>
-    <t>Created the starting form with buttons to begin types of games, added background images to both the starting form and the game board form.</t>
-  </si>
-  <si>
-    <t>Create Dealing Cards Methods</t>
-  </si>
-  <si>
-    <t>Created basic "dealer rules" AI that stands on 17 or higher and hits below that.</t>
-  </si>
-  <si>
     <t>1 hour</t>
+  </si>
+  <si>
+    <t>Created server host form and added panel to main form of game item to serve as the chat window when connecting to the server.</t>
+  </si>
+  <si>
+    <t>Revised rules and methods to prevent illogical wins/losses, prevent cross-thread errors and allow multiple rounds</t>
+  </si>
+  <si>
+    <t>Finished</t>
+  </si>
+  <si>
+    <t>Made derived class for aces with option to swap value if the value would cause the total to exceed 21.</t>
+  </si>
+  <si>
+    <t>1.5 hours</t>
+  </si>
+  <si>
+    <t>Created starting methods for server-side host to instantiate a server for users. Started on client-side connection. Working on methods to populate a combo box with the usernames of currently logged in users and transfer the connection to another form when the game begins.</t>
+  </si>
+  <si>
+    <t>Send Game Challenge via Chat</t>
+  </si>
+  <si>
+    <t>Allow a user to send a challenge via the chat system to initiate a game between players</t>
+  </si>
+  <si>
+    <t>Created challenge class, added detection to the TcpListener. Testing to ensure the message only arrives for the individual it was intended for.</t>
   </si>
 </sst>
 </file>
@@ -334,8 +343,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A2:F186" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
-  <autoFilter ref="A2:F186" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A2:F185" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="A2:F185" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Task" dataDxfId="13"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Feature" dataDxfId="12"/>
@@ -626,10 +635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,16 +692,16 @@
         <v>18</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>32</v>
       </c>
@@ -703,16 +712,16 @@
         <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="225" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>36</v>
       </c>
@@ -722,24 +731,39 @@
       <c r="C5" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="D5" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="E5" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F5" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>35</v>
@@ -748,27 +772,13 @@
         <v>18</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>